<commit_message>
✨ Commit inicial do sistema de cobranças (FastAPI + envio WhatsApp via Excel)
</commit_message>
<xml_diff>
--- a/data/saida/contatos_em_andamento.xlsx
+++ b/data/saida/contatos_em_andamento.xlsx
@@ -482,7 +482,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-08-31 11:32:15</t>
+          <t>2025-09-01 01:14:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr"/>
@@ -504,7 +504,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-08-31 11:32:58</t>
+          <t>2025-09-01 01:14:43</t>
         </is>
       </c>
       <c r="F3" t="inlineStr"/>
@@ -526,7 +526,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-08-31 11:33:41</t>
+          <t>2025-09-01 01:15:27</t>
         </is>
       </c>
       <c r="F4" t="inlineStr"/>
@@ -548,7 +548,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-08-31 11:34:25</t>
+          <t>2025-09-01 01:16:10</t>
         </is>
       </c>
       <c r="F5" t="inlineStr"/>
@@ -570,7 +570,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>2025-08-31 11:35:08</t>
+          <t>2025-09-01 01:16:54</t>
         </is>
       </c>
       <c r="F6" t="inlineStr"/>

</xml_diff>

<commit_message>
atualizando o front e backup
</commit_message>
<xml_diff>
--- a/data/saida/contatos_em_andamento.xlsx
+++ b/data/saida/contatos_em_andamento.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,139 +445,133 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>TELEFONE</t>
+          <t>NUMERO</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>RESPONDEU</t>
+          <t>valor</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>TENTATIVAS</t>
+          <t>vencimento</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>ULTIMO_ENVIO</t>
+          <t>status</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>ERRO_ULTIMO_ENVIO</t>
+          <t>STATUS</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>gustavo Barbosa pinto de souza</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>+5561994121708</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="n">
-        <v>1</v>
+          <t>Gustavo</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>619994121708</v>
+      </c>
+      <c r="C2" t="n">
+        <v>100</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>45910</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-09-01 01:14:00</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr"/>
+          <t>pendente</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>enviado</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>marcio barbosa de souza</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>+5561999890828</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="n">
-        <v>1</v>
+          <t>Gisele</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>61993367127</v>
+      </c>
+      <c r="C3" t="n">
+        <v>85</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>45912</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-09-01 01:14:43</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
+          <t>pendente</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>enviado</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>antonio ferreira pinto</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>+5561992082012</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="n">
-        <v>1</v>
+          <t>Iury</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>61993121599</v>
+      </c>
+      <c r="C4" t="n">
+        <v>90</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>45915</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>2025-09-01 01:15:27</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
+          <t>pendente</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>enviado</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Keyla barbosa Pinto</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>+5561995979443</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="n">
-        <v>1</v>
+          <t>Murillo</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>61996544168</v>
+      </c>
+      <c r="C5" t="n">
+        <v>75</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>45912</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>2025-09-01 01:16:10</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Murillo araujo jesus</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>+5561996544168</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>2025-09-01 01:16:54</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr"/>
+          <t>pendente</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>enviado</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>